<commit_message>
Comparing Sql and Elastic Importing data
</commit_message>
<xml_diff>
--- a/websiteautomation/ExcelData/CompareQueries.xlsx
+++ b/websiteautomation/ExcelData/CompareQueries.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishwa\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3FE6BC-CB03-47D8-8CDB-C6DE2938832A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1F2BAE27-E245-4FD4-8167-61193BCE2083}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{30C25F3C-84FD-4FE8-BBA5-3B806DC0B1F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="2970" xr2:uid="{30C25F3C-84FD-4FE8-BBA5-3B806DC0B1F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Mysql" sheetId="1" r:id="rId1"/>
     <sheet name="Elastic" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:D2"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Mysql Query</t>
   </si>
@@ -38,6 +34,9 @@
   </si>
   <si>
     <t>select sum(revenue),sum(quantity) from aggregation-data where date IN('2018-07-23', '2018-07-16', '2018-07-09', '2018-07-02') and product_id ='pr_5746a7a8198ef' and hub_id = 4</t>
+  </si>
+  <si>
+    <t>select count(*) from orderadataplannew</t>
   </si>
 </sst>
 </file>
@@ -434,7 +433,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>